<commit_message>
Initial commit related to advance search feature.
</commit_message>
<xml_diff>
--- a/managementcmdfiles/fdata.xlsx
+++ b/managementcmdfiles/fdata.xlsx
@@ -3478,10 +3478,10 @@
   </sheetPr>
   <dimension ref="A1:R1442"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="M313" activeCellId="0" sqref="M313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17846,7 +17846,7 @@
         <v>1</v>
       </c>
       <c r="M311" s="17" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N311" s="17" t="n">
         <v>1</v>
@@ -17940,7 +17940,7 @@
         <v>1</v>
       </c>
       <c r="M313" s="17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N313" s="17" t="n">
         <v>1</v>

</xml_diff>